<commit_message>
Testing spec extraction across rows and columns
The example framework file currently tests the ability of the codebase to import Excel values as scalars or lists across a number of rows and columns.
In general, the last scanned value overwrites any previous value attached to an item and its specification for a particular column header.
However, in the case of a compartment/characteristic components, these are appended to a list.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_example.xlsx
+++ b/tests/frameworks/framework_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Types" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -226,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -277,7 +277,7 @@
 which is a set of compartments or, recursively, other characteristics.
 While a characteristic value is typically the population size across
 a set of compartments at a point in time, it can also be normalized by
-a characteristic.
+another characteristic.
 Defining a characteristic allows the model to track other important
 system state variables beyond the size of just one compartment.
 Examples include 'Number of People Alive', 'Number of Infections Across
@@ -303,7 +303,7 @@
 which is a set of compartments or, recursively, other characteristics.
 While a characteristic value is typically the population size across
 a set of compartments at a point in time, it can also be normalized by
-a characteristic.
+another characteristic.
 Defining a characteristic allows the model to track other important
 system state variables beyond the size of just one compartment.
 Examples include 'alive', 'num_inf_all', 'prop_imm', etc.
@@ -312,6 +312,32 @@
 Note: A code name is a representative key that developers interface
 with (e.g. in scripts and the codebase).
 It should be in lower case without spaces.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column, and any that immediately follow without a specified
+header, is for the 'components' of a cascade characteristic.
+A component is either a compartment or a characteristic that has
+been previously defined, i.e. in a previous row, and should be
+listed in this (and appropriate subsequent columns) by 'Code Name'.
+For example, characteristic 'infected' may include 'dis_stage_1',
+'dis_stage_2' and 'dis_advanced', where 'dis_advanced' is another
+previously-defined characteristic including 'dis_stage_3' and
+'dis_stage_4'.
+In an example model, 'infected' would track population size summed
+across the four 'dis_stage' states.
+Note: If two or more components are listed in the same column, they
+must be separated by a comma.
+Whitespace is allowable and will be deleted during processing.</t>
         </r>
       </text>
     </comment>
@@ -390,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
   <si>
     <t>Attribute Display Name</t>
   </si>
@@ -452,262 +478,265 @@
     <t>n</t>
   </si>
   <si>
+    <t>Compartment 1</t>
+  </si>
+  <si>
+    <t>comp_1</t>
+  </si>
+  <si>
+    <t>Compartment 2</t>
+  </si>
+  <si>
+    <t>comp_2</t>
+  </si>
+  <si>
+    <t>Compartment 3</t>
+  </si>
+  <si>
+    <t>comp_3</t>
+  </si>
+  <si>
+    <t>Compartment 4</t>
+  </si>
+  <si>
+    <t>comp_4</t>
+  </si>
+  <si>
+    <t>Compartment 5</t>
+  </si>
+  <si>
+    <t>comp_5</t>
+  </si>
+  <si>
+    <t>Compartment 6</t>
+  </si>
+  <si>
+    <t>comp_6</t>
+  </si>
+  <si>
+    <t>Compartment 7</t>
+  </si>
+  <si>
+    <t>comp_7</t>
+  </si>
+  <si>
+    <t>Compartment 8</t>
+  </si>
+  <si>
+    <t>comp_8</t>
+  </si>
+  <si>
+    <t>Compartment 9</t>
+  </si>
+  <si>
+    <t>comp_9</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Characteristic 0</t>
+  </si>
+  <si>
+    <t>charac_0</t>
+  </si>
+  <si>
+    <t>Characteristic 1</t>
+  </si>
+  <si>
+    <t>charac_1</t>
+  </si>
+  <si>
+    <t>Characteristic 2</t>
+  </si>
+  <si>
+    <t>charac_2</t>
+  </si>
+  <si>
+    <t>Characteristic 3</t>
+  </si>
+  <si>
+    <t>charac_3</t>
+  </si>
+  <si>
+    <t>Characteristic 4</t>
+  </si>
+  <si>
+    <t>charac_4</t>
+  </si>
+  <si>
+    <t>Characteristic 5</t>
+  </si>
+  <si>
+    <t>charac_5</t>
+  </si>
+  <si>
+    <t>Characteristic 6</t>
+  </si>
+  <si>
+    <t>charac_6</t>
+  </si>
+  <si>
+    <t>Transition Tag</t>
+  </si>
+  <si>
+    <t>Parameter 0</t>
+  </si>
+  <si>
+    <t>par_0</t>
+  </si>
+  <si>
+    <t>Parameter 1</t>
+  </si>
+  <si>
+    <t>par_1</t>
+  </si>
+  <si>
+    <t>Parameter 2</t>
+  </si>
+  <si>
+    <t>par_2</t>
+  </si>
+  <si>
+    <t>Parameter 3</t>
+  </si>
+  <si>
+    <t>par_3</t>
+  </si>
+  <si>
+    <t>Parameter 4</t>
+  </si>
+  <si>
+    <t>par_4</t>
+  </si>
+  <si>
+    <t>Parameter 5</t>
+  </si>
+  <si>
+    <t>par_5</t>
+  </si>
+  <si>
+    <t>Parameter 6</t>
+  </si>
+  <si>
+    <t>par_6</t>
+  </si>
+  <si>
+    <t>Parameter 7</t>
+  </si>
+  <si>
+    <t>par_7</t>
+  </si>
+  <si>
+    <t>Parameter 8</t>
+  </si>
+  <si>
+    <t>par_8</t>
+  </si>
+  <si>
+    <t>Parameter 9</t>
+  </si>
+  <si>
+    <t>par_9</t>
+  </si>
+  <si>
+    <t>Parameter 10</t>
+  </si>
+  <si>
+    <t>par_10</t>
+  </si>
+  <si>
+    <t>Parameter 11</t>
+  </si>
+  <si>
+    <t>par_11</t>
+  </si>
+  <si>
+    <t>Parameter 12</t>
+  </si>
+  <si>
+    <t>par_12</t>
+  </si>
+  <si>
+    <t>Parameter 13</t>
+  </si>
+  <si>
+    <t>par_13</t>
+  </si>
+  <si>
+    <t>Parameter 14</t>
+  </si>
+  <si>
+    <t>par_14</t>
+  </si>
+  <si>
+    <t>Parameter 15</t>
+  </si>
+  <si>
+    <t>par_15</t>
+  </si>
+  <si>
+    <t>Parameter 16</t>
+  </si>
+  <si>
+    <t>par_16</t>
+  </si>
+  <si>
+    <t>Parameter 17</t>
+  </si>
+  <si>
+    <t>par_17</t>
+  </si>
+  <si>
+    <t>Parameter 18</t>
+  </si>
+  <si>
+    <t>par_18</t>
+  </si>
+  <si>
+    <t>Parameter 19</t>
+  </si>
+  <si>
+    <t>par_19</t>
+  </si>
+  <si>
+    <t>Program Type 0</t>
+  </si>
+  <si>
+    <t>progtype_0</t>
+  </si>
+  <si>
+    <t>Program Type 1</t>
+  </si>
+  <si>
+    <t>progtype_1</t>
+  </si>
+  <si>
+    <t>Program Type 2</t>
+  </si>
+  <si>
+    <t>progtype_2</t>
+  </si>
+  <si>
+    <t>Program Type 3</t>
+  </si>
+  <si>
+    <t>progtype_3</t>
+  </si>
+  <si>
+    <t>Program Type 4</t>
+  </si>
+  <si>
+    <t>progtype_4</t>
+  </si>
+  <si>
+    <t>Program Type 5</t>
+  </si>
+  <si>
+    <t>progtype_5</t>
+  </si>
+  <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>Compartment 1</t>
-  </si>
-  <si>
-    <t>comp_1</t>
-  </si>
-  <si>
-    <t>Compartment 2</t>
-  </si>
-  <si>
-    <t>comp_2</t>
-  </si>
-  <si>
-    <t>Compartment 3</t>
-  </si>
-  <si>
-    <t>comp_3</t>
-  </si>
-  <si>
-    <t>Compartment 4</t>
-  </si>
-  <si>
-    <t>comp_4</t>
-  </si>
-  <si>
-    <t>Compartment 5</t>
-  </si>
-  <si>
-    <t>comp_5</t>
-  </si>
-  <si>
-    <t>Compartment 6</t>
-  </si>
-  <si>
-    <t>comp_6</t>
-  </si>
-  <si>
-    <t>Compartment 7</t>
-  </si>
-  <si>
-    <t>comp_7</t>
-  </si>
-  <si>
-    <t>Compartment 8</t>
-  </si>
-  <si>
-    <t>comp_8</t>
-  </si>
-  <si>
-    <t>Compartment 9</t>
-  </si>
-  <si>
-    <t>comp_9</t>
-  </si>
-  <si>
-    <t>Characteristic 0</t>
-  </si>
-  <si>
-    <t>charac_0</t>
-  </si>
-  <si>
-    <t>Characteristic 1</t>
-  </si>
-  <si>
-    <t>charac_1</t>
-  </si>
-  <si>
-    <t>Characteristic 2</t>
-  </si>
-  <si>
-    <t>charac_2</t>
-  </si>
-  <si>
-    <t>Characteristic 3</t>
-  </si>
-  <si>
-    <t>charac_3</t>
-  </si>
-  <si>
-    <t>Characteristic 4</t>
-  </si>
-  <si>
-    <t>charac_4</t>
-  </si>
-  <si>
-    <t>Characteristic 5</t>
-  </si>
-  <si>
-    <t>charac_5</t>
-  </si>
-  <si>
-    <t>Characteristic 6</t>
-  </si>
-  <si>
-    <t>charac_6</t>
-  </si>
-  <si>
-    <t>Transition Tag</t>
-  </si>
-  <si>
-    <t>Parameter 0</t>
-  </si>
-  <si>
-    <t>par_0</t>
-  </si>
-  <si>
-    <t>Parameter 1</t>
-  </si>
-  <si>
-    <t>par_1</t>
-  </si>
-  <si>
-    <t>Parameter 2</t>
-  </si>
-  <si>
-    <t>par_2</t>
-  </si>
-  <si>
-    <t>Parameter 3</t>
-  </si>
-  <si>
-    <t>par_3</t>
-  </si>
-  <si>
-    <t>Parameter 4</t>
-  </si>
-  <si>
-    <t>par_4</t>
-  </si>
-  <si>
-    <t>Parameter 5</t>
-  </si>
-  <si>
-    <t>par_5</t>
-  </si>
-  <si>
-    <t>Parameter 6</t>
-  </si>
-  <si>
-    <t>par_6</t>
-  </si>
-  <si>
-    <t>Parameter 7</t>
-  </si>
-  <si>
-    <t>par_7</t>
-  </si>
-  <si>
-    <t>Parameter 8</t>
-  </si>
-  <si>
-    <t>par_8</t>
-  </si>
-  <si>
-    <t>Parameter 9</t>
-  </si>
-  <si>
-    <t>par_9</t>
-  </si>
-  <si>
-    <t>Parameter 10</t>
-  </si>
-  <si>
-    <t>par_10</t>
-  </si>
-  <si>
-    <t>Parameter 11</t>
-  </si>
-  <si>
-    <t>par_11</t>
-  </si>
-  <si>
-    <t>Parameter 12</t>
-  </si>
-  <si>
-    <t>par_12</t>
-  </si>
-  <si>
-    <t>Parameter 13</t>
-  </si>
-  <si>
-    <t>par_13</t>
-  </si>
-  <si>
-    <t>Parameter 14</t>
-  </si>
-  <si>
-    <t>par_14</t>
-  </si>
-  <si>
-    <t>Parameter 15</t>
-  </si>
-  <si>
-    <t>par_15</t>
-  </si>
-  <si>
-    <t>Parameter 16</t>
-  </si>
-  <si>
-    <t>par_16</t>
-  </si>
-  <si>
-    <t>Parameter 17</t>
-  </si>
-  <si>
-    <t>par_17</t>
-  </si>
-  <si>
-    <t>Parameter 18</t>
-  </si>
-  <si>
-    <t>par_18</t>
-  </si>
-  <si>
-    <t>Parameter 19</t>
-  </si>
-  <si>
-    <t>par_19</t>
-  </si>
-  <si>
-    <t>Program Type 0</t>
-  </si>
-  <si>
-    <t>progtype_0</t>
-  </si>
-  <si>
-    <t>Program Type 1</t>
-  </si>
-  <si>
-    <t>progtype_1</t>
-  </si>
-  <si>
-    <t>Program Type 2</t>
-  </si>
-  <si>
-    <t>progtype_2</t>
-  </si>
-  <si>
-    <t>Program Type 3</t>
-  </si>
-  <si>
-    <t>progtype_3</t>
-  </si>
-  <si>
-    <t>Program Type 4</t>
-  </si>
-  <si>
-    <t>progtype_4</t>
-  </si>
-  <si>
-    <t>Program Type 5</t>
-  </si>
-  <si>
-    <t>progtype_5</t>
   </si>
   <si>
     <t>blug</t>
@@ -1281,18 +1310,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="5" width="15.73046875" customWidth="1"/>
+    <col min="1" max="6" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1302,14 +1331,15 @@
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1317,180 +1347,258 @@
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>106</v>
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D11" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C19 E2:F19 D2:D16 D18:D19" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"n,y"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10" xr:uid="{00000000-0002-0000-0100-000002000000}">
-      <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1508,77 +1616,119 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="20.73046875" customWidth="1"/>
+    <col min="1" max="3" width="20.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" s="2" t="str">
+        <f>CONCATENATE(Compartments!B2)</f>
+        <v>comp_0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" s="2" t="str">
+        <f>CONCATENATE(Compartments!B4,", ",B2)</f>
+        <v>comp_1, charac_0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="2" t="str">
+        <f>CONCATENATE(Compartments!B10,", ",B5)</f>
+        <v>comp_4, charac_3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="2" t="str">
+        <f>CONCATENATE(Compartments!B12,", ",B7)</f>
+        <v>comp_5, charac_4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>52</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f>CONCATENATE(Compartments!B14,", ",B8)</f>
+        <v>comp_6, charac_5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Semantic overhaul for item type
This commit establishes a clear distinction between individual framework items in a framework file, e.g. a compartment, versus the type of the item, e.g. the compartment type.
The latter revolves around IO interpretation definitions and is stored in FrameworkSettings, while the former is part of a model skeleton and is stored in ProjectFramework.
This distinction between metadata and metametadata is subtle but vital and avoids namespace collisions.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_example.xlsx
+++ b/tests/frameworks/framework_example.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Population Types" sheetId="1" r:id="rId1"/>
+    <sheet name="Population Attributes" sheetId="1" r:id="rId1"/>
     <sheet name="Compartments" sheetId="2" r:id="rId2"/>
     <sheet name="Transitions" sheetId="3" r:id="rId3"/>
     <sheet name="Characteristics" sheetId="4" r:id="rId4"/>
@@ -1137,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1618,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>